<commit_message>
changed setting, fixed to send map data
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C-Sync\Naver MYBOX\문서\Multi-3D-PacMan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wltjd\OneDrive\바탕 화면\2021 2학기 강의자료\네트워크프로그래밍\TeamProject\Multi-3D-PacMan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0246CB72-8EFA-44D9-8C2F-31CFAD0E5B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7333AEB1-5EAF-4724-B6C6-B777FF516534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CA08BBB5-14F5-460E-B4ED-A4EB4C70ABF3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CA08BBB5-14F5-460E-B4ED-A4EB4C70ABF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="87">
   <si>
     <t>2일</t>
   </si>
@@ -515,17 +515,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0070C0"/>
       <name val="맑은 고딕"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -737,14 +738,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1067,7 +1068,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1078,32 +1079,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808FE5DC-E203-4BDA-A160-15A588217312}">
   <dimension ref="A3:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.69921875" customWidth="1"/>
-    <col min="2" max="2" width="42.19921875" customWidth="1"/>
-    <col min="3" max="3" width="13.8984375" customWidth="1"/>
-    <col min="4" max="4" width="41.09765625" customWidth="1"/>
-    <col min="5" max="5" width="13.3984375" customWidth="1"/>
-    <col min="6" max="6" width="42.09765625" customWidth="1"/>
-    <col min="7" max="7" width="27.19921875" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="42.25" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="41.125" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="42.125" customWidth="1"/>
+    <col min="7" max="7" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="33.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>50</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>51</v>
       </c>
@@ -1143,7 +1144,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -1179,7 +1180,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
@@ -1191,7 +1192,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1206,7 +1207,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1221,7 @@
       <c r="E10" s="2"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>7</v>
       </c>
@@ -1237,7 +1238,7 @@
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
@@ -1248,7 +1249,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
@@ -1265,7 +1266,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>10</v>
       </c>
@@ -1277,7 +1278,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1292,7 +1293,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
@@ -1304,7 +1305,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>13</v>
       </c>
@@ -1314,7 +1315,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>14</v>
       </c>
@@ -1331,7 +1332,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>15</v>
       </c>
@@ -1343,7 +1344,7 @@
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>16</v>
       </c>
@@ -1357,7 +1358,7 @@
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>17</v>
       </c>
@@ -1372,7 +1373,7 @@
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1388,7 @@
       <c r="F22" s="15"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>19</v>
       </c>
@@ -1402,7 +1403,7 @@
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>20</v>
       </c>
@@ -1412,7 +1413,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>21</v>
       </c>
@@ -1429,7 +1430,7 @@
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>22</v>
       </c>
@@ -1440,7 +1441,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>23</v>
       </c>
@@ -1455,7 +1456,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>24</v>
       </c>
@@ -1468,7 +1469,7 @@
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>25</v>
       </c>
@@ -1483,7 +1484,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>26</v>
       </c>
@@ -1496,7 +1497,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>27</v>
       </c>
@@ -1506,7 +1507,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>28</v>
       </c>
@@ -1523,7 +1524,7 @@
       </c>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>52</v>
       </c>
@@ -1534,7 +1535,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1544,7 @@
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>1</v>
       </c>
@@ -1552,14 +1553,14 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="2"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>3</v>
       </c>
@@ -1570,7 +1571,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>4</v>
       </c>
@@ -1587,7 +1588,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>5</v>
       </c>
@@ -1598,7 +1599,7 @@
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1607,16 +1608,16 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="33.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="23" t="s">
+    <row r="41" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:7" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>50</v>
       </c>
@@ -1639,7 +1640,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="42" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" ht="42" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>51</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>44</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="21" t="s">
         <v>32</v>
       </c>
       <c r="E43" s="2"/>
@@ -1656,7 +1657,7 @@
       </c>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>2</v>
       </c>
@@ -1666,7 +1667,7 @@
       <c r="C44" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="21" t="s">
         <v>53</v>
       </c>
       <c r="E44" s="2"/>
@@ -1677,7 +1678,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>3</v>
       </c>
@@ -1685,31 +1686,31 @@
         <v>81</v>
       </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="22"/>
+      <c r="D45" s="21"/>
       <c r="E45" s="2"/>
       <c r="F45" s="20" t="s">
         <v>79</v>
       </c>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E46" s="2"/>
-      <c r="F46" s="21" t="s">
+      <c r="F46" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>5</v>
       </c>
@@ -1719,16 +1720,16 @@
       <c r="C47" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1739,7 @@
       <c r="C48" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="24" t="s">
         <v>56</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -1746,24 +1747,13 @@
       </c>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G49" s="5"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>8</v>
       </c>
@@ -1774,7 +1764,7 @@
       </c>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>9</v>
       </c>
@@ -1791,7 +1781,7 @@
       </c>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>10</v>
       </c>
@@ -1803,7 +1793,7 @@
       </c>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>11</v>
       </c>
@@ -1818,7 +1808,7 @@
       </c>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1820,7 @@
       </c>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>13</v>
       </c>
@@ -1840,7 +1830,7 @@
       <c r="F55" s="15"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>14</v>
       </c>
@@ -1857,7 +1847,7 @@
       </c>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>15</v>
       </c>
@@ -1869,7 +1859,7 @@
       </c>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>16</v>
       </c>
@@ -1883,7 +1873,7 @@
       </c>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>17</v>
       </c>
@@ -1898,7 +1888,7 @@
       </c>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>18</v>
       </c>
@@ -1913,7 +1903,7 @@
       <c r="F60" s="15"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>19</v>
       </c>
@@ -1928,7 +1918,7 @@
       </c>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>20</v>
       </c>
@@ -1938,7 +1928,7 @@
       <c r="F62" s="2"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>21</v>
       </c>
@@ -1955,7 +1945,7 @@
       </c>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
         <v>22</v>
       </c>
@@ -1966,7 +1956,7 @@
       <c r="F64" s="2"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>23</v>
       </c>
@@ -1981,7 +1971,7 @@
       </c>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>24</v>
       </c>
@@ -1994,7 +1984,7 @@
       </c>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +1999,7 @@
       <c r="F67" s="2"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>26</v>
       </c>
@@ -2022,7 +2012,7 @@
       <c r="F68" s="2"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>27</v>
       </c>
@@ -2032,7 +2022,7 @@
       <c r="F69" s="2"/>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>28</v>
       </c>
@@ -2049,7 +2039,7 @@
       </c>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>52</v>
       </c>
@@ -2060,7 +2050,7 @@
       <c r="F71" s="2"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>0</v>
       </c>
@@ -2069,7 +2059,7 @@
       </c>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>1</v>
       </c>
@@ -2078,14 +2068,14 @@
       </c>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B74" s="2"/>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>3</v>
       </c>
@@ -2096,7 +2086,7 @@
       <c r="F75" s="2"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2103,7 @@
       </c>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="12" t="s">
         <v>5</v>
       </c>
@@ -2124,7 +2114,7 @@
       <c r="F77" s="8"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="78" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:F3"/>

</xml_diff>

<commit_message>
[FIX] Progress Report 재수정
</commit_message>
<xml_diff>
--- a/Progress Report.xlsx
+++ b/Progress Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\C-Sync\Naver MYBOX\문서\Multi-3D-PacMan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434DF2E5-A4AE-40FD-842B-5165050DF177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9BFB71-4525-4C85-BEF5-C8581A248E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CA08BBB5-14F5-460E-B4ED-A4EB4C70ABF3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="101">
   <si>
     <t>2일</t>
   </si>
@@ -405,10 +405,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Send, Recv 구현</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>서버 클래스 생성 및 함수 정의
 예외 처리 클래스</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -564,15 +560,24 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>네트워크 쪽에서 맵 관련 작업 수정 완료</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>클라이언트 작업 오류 수정(깃 머지하면서 추가된 작업)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>맵 받아서 그리기, 클라이언트 구조 수정(함수 등 네트워크 라이브러리에 있는 걸로 변경),  최신화된 서버반영</t>
+    <t>스레드 함수 생성 및 수신 기능 구현 
+클라 Send, Recv 구현</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵 받아서 그리기, 클라이언트 구조 수정(함수 등 네트워크 라이브러리에 있는 걸로 변경)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">네트워크에서 맵 수정 필요 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>네트워크에서 맵 수정 완료</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -707,7 +712,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -727,6 +732,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -845,7 +856,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -927,16 +938,25 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1271,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808FE5DC-E203-4BDA-A160-15A588217312}">
   <dimension ref="A3:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1288,13 +1308,13 @@
   <sheetData>
     <row r="3" spans="1:7" ht="33.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:7" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
@@ -1490,7 +1510,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
@@ -1507,12 +1527,12 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -1580,7 +1600,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
@@ -1597,7 +1617,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
@@ -1829,13 +1849,13 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="33.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:7" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
@@ -1873,7 +1893,7 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G43" s="3"/>
     </row>
@@ -1928,16 +1948,14 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A47" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="B47" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="22" t="s">
         <v>34</v>
       </c>
@@ -1950,16 +1968,16 @@
         <v>6</v>
       </c>
       <c r="B48" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>55</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G48" s="3"/>
     </row>
@@ -1967,19 +1985,25 @@
       <c r="A49" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="3"/>
+      <c r="B49" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="31"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="E50" s="2"/>
       <c r="F50" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G50" s="3"/>
     </row>
@@ -1987,18 +2011,18 @@
       <c r="A51" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>97</v>
+      <c r="C51" t="s">
+        <v>100</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.4">
@@ -2011,12 +2035,12 @@
       </c>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A53" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="16" t="s">
-        <v>99</v>
+      <c r="B53" s="20" t="s">
+        <v>98</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
@@ -2027,7 +2051,7 @@
         <v>65</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -2037,7 +2061,7 @@
       <c r="C54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -2048,7 +2072,7 @@
       <c r="C55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G55" s="3"/>
     </row>
@@ -2056,16 +2080,20 @@
       <c r="A56" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="G56" s="3"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" s="31"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="33" t="s">
         <v>35</v>
       </c>
       <c r="C57" s="2"/>
@@ -2108,7 +2136,7 @@
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
@@ -2125,7 +2153,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">

</xml_diff>